<commit_message>
Corrected Bug in Code
</commit_message>
<xml_diff>
--- a/Exported_Case_Arrival.xlsx
+++ b/Exported_Case_Arrival.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\Corona Virus\Coronavirus-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED7DBE6-0FE2-4DC7-B00D-30EC78E6C80E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90BD92A-0449-4934-94A4-0E14B53364C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
   <si>
     <t>Country</t>
   </si>
@@ -296,6 +296,18 @@
   </si>
   <si>
     <t>Arrival date to date of symptom onset</t>
+  </si>
+  <si>
+    <t>https://www.who.int/csr/don/21-january-2020-novel-coronavirus-republic-of-korea-ex-china/en/,http://www.chinacdc.cn/en/,https://shimo.im/sheets/tyWrrrqppYVwQtCW/oURp4/?from=singlemessage&amp;isappinstalled=0</t>
+  </si>
+  <si>
+    <t>https://www.cdc.go.kr/cdc_eng/,http://www.chinacdc.cn/en/,https://shimo.im/sheets/tyWrrrqppYVwQtCW/oURp4/?from=singlemessage&amp;isappinstalled=0</t>
+  </si>
+  <si>
+    <t>https://www.mhlw.go.jp/english/,http://www.chinacdc.cn/en/,https://shimo.im/sheets/tyWrrrqppYVwQtCW/oURp4/?from=singlemessage&amp;isappinstalled=0</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/En,http://www.chinacdc.cn/en/,https://shimo.im/sheets/tyWrrrqppYVwQtCW/oURp4/?from=singlemessage&amp;isappinstalled=0</t>
   </si>
 </sst>
 </file>
@@ -308,7 +320,7 @@
     <numFmt numFmtId="166" formatCode="mmmm&quot; &quot;d&quot;, &quot;yyyy"/>
     <numFmt numFmtId="167" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -385,16 +397,6 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambira"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Cambira"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -446,7 +448,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -480,8 +482,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -500,6 +500,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -507,7 +508,21 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -738,11 +753,11 @@
   </sheetPr>
   <dimension ref="A1:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -753,29 +768,29 @@
     <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:28" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:28" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" ht="13.5" thickBot="1">
+    <row r="3" spans="1:28" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -788,7 +803,7 @@
       <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>79</v>
       </c>
       <c r="F3" s="13" t="s">
@@ -819,7 +834,7 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
     </row>
-    <row r="4" spans="1:28" ht="14.25">
+    <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
@@ -839,9 +854,11 @@
       <c r="F4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:28" ht="14.25">
+      <c r="G4" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -861,30 +878,34 @@
       <c r="F5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:28" s="24" customFormat="1" ht="14.25">
-      <c r="A6" s="25" t="s">
+      <c r="G5" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="10" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="24">
         <v>43850</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="24">
         <v>43850</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="24">
         <v>43856</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>0</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:28" ht="14.25">
+      <c r="G6" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>9</v>
       </c>
@@ -904,9 +925,11 @@
       <c r="F7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:28" ht="14.25">
+      <c r="G7" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
@@ -926,9 +949,11 @@
       <c r="F8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:28" ht="14.25">
+      <c r="G8" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
@@ -948,9 +973,11 @@
       <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:28" ht="14.25">
+      <c r="G9" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
@@ -970,9 +997,11 @@
       <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:28" ht="14.25">
+      <c r="G10" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
@@ -987,9 +1016,11 @@
       <c r="F11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:28" ht="14.25">
+      <c r="G11" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
@@ -1009,9 +1040,11 @@
       <c r="F12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:28" ht="14.25">
+      <c r="G12" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>7</v>
       </c>
@@ -1031,9 +1064,11 @@
       <c r="F13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="1:28" ht="14.25">
+      <c r="G13" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1048,9 +1083,11 @@
       <c r="F14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="1:28" ht="14.25">
+      <c r="G14" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>10</v>
       </c>
@@ -1070,9 +1107,11 @@
       <c r="F15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:28" ht="14.25">
+      <c r="G15" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>10</v>
       </c>
@@ -1092,9 +1131,11 @@
       <c r="F16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:7" ht="14.25">
+      <c r="G16" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>10</v>
       </c>
@@ -1114,9 +1155,11 @@
       <c r="F17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="1:7" ht="14.25">
+      <c r="G17" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>10</v>
       </c>
@@ -1136,9 +1179,11 @@
       <c r="F18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" ht="14.25">
+      <c r="G18" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>10</v>
       </c>
@@ -1158,9 +1203,11 @@
       <c r="F19" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" ht="14.25">
+      <c r="G19" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>10</v>
       </c>
@@ -1180,9 +1227,11 @@
       <c r="F20" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" ht="14.25">
+      <c r="G20" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>10</v>
       </c>
@@ -1202,9 +1251,11 @@
       <c r="F21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G21" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1274,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1298,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>2</v>
       </c>
@@ -1264,7 +1315,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>53</v>
       </c>
@@ -1284,7 +1335,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.25">
+    <row r="26" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1355,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.25">
+    <row r="27" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
@@ -1321,7 +1372,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.25">
+    <row r="28" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>32</v>
       </c>
@@ -1340,7 +1391,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.25">
+    <row r="29" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>12</v>
       </c>
@@ -1360,7 +1411,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.25">
+    <row r="30" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
         <v>8</v>
       </c>
@@ -1382,7 +1433,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="14.25">
+    <row r="31" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>4</v>
       </c>
@@ -1404,7 +1455,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.25">
+    <row r="32" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
         <v>1</v>
       </c>
@@ -1419,7 +1470,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14.25">
+    <row r="33" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>1</v>
       </c>
@@ -1437,7 +1488,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:7" ht="14.25">
+    <row r="34" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
         <v>1</v>
       </c>
@@ -1454,7 +1505,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.25">
+    <row r="35" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>11</v>
       </c>
@@ -1474,7 +1525,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="14.25">
+    <row r="36" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14.25">
+    <row r="37" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>3</v>
       </c>
@@ -1509,7 +1560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14.25">
+    <row r="38" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
         <v>42</v>
       </c>
@@ -1526,7 +1577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="14.25">
+    <row r="39" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
         <v>44</v>
       </c>
@@ -1543,7 +1594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="14.25">
+    <row r="40" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
         <v>46</v>
       </c>
@@ -1560,7 +1611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="14.25">
+    <row r="41" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>48</v>
       </c>
@@ -1580,7 +1631,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.25">
+    <row r="42" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
         <v>50</v>
       </c>
@@ -1600,7 +1651,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="14.25">
+    <row r="43" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>33</v>
       </c>
@@ -1615,7 +1666,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.25">
+    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
         <v>53</v>
       </c>
@@ -1630,7 +1681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.25">
+    <row r="45" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>33</v>
       </c>
@@ -1645,7 +1696,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.25">
+    <row r="46" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>56</v>
       </c>
@@ -1660,7 +1711,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="14.25">
+    <row r="47" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>58</v>
       </c>
@@ -1675,7 +1726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="12.75">
+    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="20"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -1686,141 +1737,141 @@
       </c>
       <c r="G48" s="20"/>
     </row>
-    <row r="49" spans="1:5" ht="12.75">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" ht="12.75">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" ht="12.75">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" ht="12.75">
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="12.75">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="5"/>
       <c r="C53" s="6"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="12.75">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="5"/>
       <c r="C54" s="6"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:5" ht="12.75">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="5"/>
       <c r="C55" s="6"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5" ht="12.75">
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="5"/>
       <c r="C56" s="6"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="1:5" ht="12.75">
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="5"/>
       <c r="C57" s="6"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5" ht="12.75">
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="5"/>
       <c r="C58" s="6"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="1:5" ht="12.75">
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="C59" s="6"/>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="1:5" ht="12.75">
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="C60" s="4"/>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:5" ht="12.75">
+    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="12.75">
+    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:5" ht="12.75">
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" ht="12.75">
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" ht="12.75">
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" ht="12.75">
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" ht="12.75">
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:5" ht="12.75">
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="C68" s="4"/>
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="1:5" ht="12.75">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1833,12 +1884,12 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:G5 A7:G47 G6">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$E4&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:XFD6">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A6:G6">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E6&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1862,9 +1913,27 @@
     <hyperlink ref="G45" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
     <hyperlink ref="G46" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
     <hyperlink ref="G47" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
+    <hyperlink ref="G4" r:id="rId20" xr:uid="{34A0EC33-430D-4FA2-B9FB-D1768AD7670C}"/>
+    <hyperlink ref="G5" r:id="rId21" xr:uid="{2C6BAB03-E1BF-4AFA-A9C7-0C9268462E03}"/>
+    <hyperlink ref="G6" r:id="rId22" xr:uid="{C297B8A6-62EC-4310-BD16-3AD9D88D6D91}"/>
+    <hyperlink ref="G7" r:id="rId23" xr:uid="{B7CFF5B1-747B-4D8F-8A4E-27FAD491CA71}"/>
+    <hyperlink ref="G8" r:id="rId24" xr:uid="{21A81E3B-1679-4D41-9BBA-2514BDC8B573}"/>
+    <hyperlink ref="G9" r:id="rId25" xr:uid="{7FA7C1E1-CB57-4336-8AE7-04201C8FB93C}"/>
+    <hyperlink ref="G10" r:id="rId26" xr:uid="{A0D8099E-DE51-439C-A6ED-6CFE3F41EC55}"/>
+    <hyperlink ref="G11" r:id="rId27" xr:uid="{246EC24B-2C42-430B-81A8-E6F0ADF0AB18}"/>
+    <hyperlink ref="G12" r:id="rId28" xr:uid="{F0E6499A-A868-459D-9DC5-BF100F69E320}"/>
+    <hyperlink ref="G13" r:id="rId29" xr:uid="{BF605D6B-62DB-4714-8662-31A4BC36F584}"/>
+    <hyperlink ref="G14" r:id="rId30" xr:uid="{52795501-CE15-4A71-A642-26254691F8D2}"/>
+    <hyperlink ref="G15" r:id="rId31" xr:uid="{A981857D-D908-4138-89D3-1B3F633CDD08}"/>
+    <hyperlink ref="G16" r:id="rId32" xr:uid="{1D8F2035-4100-4256-B27F-8AD2398EC5A1}"/>
+    <hyperlink ref="G17" r:id="rId33" xr:uid="{2B61AEB0-4D83-4D84-ADBD-B68C6F6F00AE}"/>
+    <hyperlink ref="G18" r:id="rId34" xr:uid="{04E44B05-BA8C-45AC-8C4E-630FE884449E}"/>
+    <hyperlink ref="G19" r:id="rId35" xr:uid="{F2AD0A6E-4882-40E7-A3EE-1A1C6616A729}"/>
+    <hyperlink ref="G20" r:id="rId36" xr:uid="{12007DD4-8BF2-4986-8C54-C05C9B9EF1FC}"/>
+    <hyperlink ref="G21" r:id="rId37" xr:uid="{24F71A93-EBCD-47DC-81FC-FE1C5F51C55A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
-  <legacyDrawing r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>